<commit_message>
docment commit on 20230918
</commit_message>
<xml_diff>
--- a/03.設計/詳細設計書_STB06（ITEM）.xlsx
+++ b/03.設計/詳細設計書_STB06（ITEM）.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
   <si>
     <t>プロジェクト番号</t>
     <rPh sb="6" eb="8">
@@ -314,133 +314,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>・上記以外の場合</t>
-    <rPh sb="1" eb="5">
-      <t>ジョウキイガイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>・赤プレイヤー かつ 移動方向が壁の場合</t>
-    <rPh sb="1" eb="2">
-      <t>アカ</t>
-    </rPh>
-    <rPh sb="11" eb="15">
-      <t>イドウホウコウ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>カベ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>・移動方向が壁、端の壁以外の場合</t>
-    <rPh sb="1" eb="5">
-      <t>イドウホウコウ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>カベ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ハシ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>カベ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>・ヒット時のSEを再生</t>
-    <rPh sb="4" eb="5">
-      <t>ジ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>サイセイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>・壁ブロックを通路に変更</t>
-    <rPh sb="1" eb="2">
-      <t>カベ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ツウロ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヘンコウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>・壁破壊ポイント数を -1 する</t>
-    <rPh sb="1" eb="2">
-      <t>カベ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ハカイ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>スウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>・壁破壊ポイント数が0の場合</t>
-    <rPh sb="1" eb="4">
-      <t>カベハカイ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>スウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>・アイテムの効果を無効化する（）</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>キー入力が左の場合</t>
-    <rPh sb="2" eb="4">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ヒダリ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>・プレイヤーのX軸座標を -1 する</t>
-    <rPh sb="8" eb="9">
-      <t>ジク</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ザヒョウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>詳細設計書_06_ITEM</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -658,6 +531,210 @@
   </si>
   <si>
     <t>TM</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>・アイテム使用判定フラグをTrueに設定</t>
+    <rPh sb="5" eb="9">
+      <t>シヨウハンテイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>・所持アイテム数（配列）の該当要素を -1 する</t>
+    <rPh sb="13" eb="15">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヨウソ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>・使用中の別のアイテム効果を無効化する（06_ITEM.&lt;アイテム無効化&gt;）</t>
+    <rPh sb="1" eb="4">
+      <t>シヨウチュウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>コウカ</t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t>ムコウカ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ムコウ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>バ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>&lt;アイテム無効化&gt;</t>
+    <rPh sb="5" eb="8">
+      <t>ムコウカ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>使用中のアイテムを無効化する</t>
+    <rPh sb="0" eb="3">
+      <t>シヨウチュウ</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>ムコウカ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>アイテム情報</t>
+    <rPh sb="4" eb="6">
+      <t>ジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>アイテム使用判定フラグ</t>
+    <rPh sb="4" eb="8">
+      <t>シヨウハンテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>設定値</t>
+    <rPh sb="0" eb="3">
+      <t>セッテイチ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>False</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>アイテム使用時間</t>
+    <rPh sb="4" eb="8">
+      <t>シヨウジカン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>プレイヤーカラー</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>黒</t>
+    <rPh sb="0" eb="1">
+      <t>クロ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>視界制限</t>
+    <rPh sb="0" eb="4">
+      <t>シカイセイゲン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>&lt;アイテム生成判定&gt;</t>
+    <rPh sb="5" eb="9">
+      <t>セイセイハンテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>フィールド上のアイテム数をカウント</t>
+    <rPh sb="5" eb="6">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>スウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>2.</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>・1でカウントしたアイテム数がアイテム最大値未満 かつ アイテム再生成クールタイムが1以上の場合</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>生成判定</t>
+    <rPh sb="0" eb="4">
+      <t>セイセイハンテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>・アイテム再生成クールタイムを -1 する</t>
+    <rPh sb="5" eb="8">
+      <t>サイセイセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>・1でカウントしたアイテム数がアイテム最大値未満 かつ アイテム再生成クールタイムが0の場合</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>・フィールド上にアイテムを生成（09_SGS.&lt;オブジェクトセット&gt;）</t>
+    <rPh sb="6" eb="7">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>セイセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>・アイテム再生成クールタイムを15秒に設定する</t>
+    <rPh sb="5" eb="8">
+      <t>サイセイセイ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ビョウ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>&lt;アイテム種類番号取得&gt;</t>
+    <rPh sb="5" eb="11">
+      <t>シュルイバンゴウシュトク</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>引数：</t>
+    <rPh sb="0" eb="2">
+      <t>ヒキスウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>アイテム番号</t>
+    <rPh sb="4" eb="6">
+      <t>バンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[小数点以下の数字-1]を抽出</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -748,7 +825,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,12 +841,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,7 +1139,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1262,7 +1333,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1271,13 +1348,7 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1396,6 +1467,12 @@
     </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1794,7 +1871,7 @@
     <row r="7" spans="3:16" ht="49.2" customHeight="1">
       <c r="C7" s="7"/>
       <c r="D7" s="74" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E7" s="74"/>
       <c r="F7" s="74"/>
@@ -1882,7 +1959,7 @@
       </c>
       <c r="G15" s="76"/>
       <c r="H15" s="77" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="I15" s="78"/>
       <c r="J15" s="78"/>
@@ -2083,7 +2160,7 @@
       </c>
       <c r="C5" s="84"/>
       <c r="D5" s="85" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E5" s="85"/>
       <c r="F5" s="85" t="s">
@@ -2577,11 +2654,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ69"/>
+  <dimension ref="A1:AJ56"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q27" sqref="Q27"/>
+      <selection pane="bottomLeft" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -2753,7 +2830,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="G5" s="17"/>
       <c r="H5" s="19"/>
@@ -2773,7 +2850,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="19"/>
@@ -2793,7 +2870,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="19"/>
@@ -2813,7 +2890,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="19"/>
@@ -3167,7 +3244,7 @@
     </row>
     <row r="18" spans="1:36" ht="15" customHeight="1">
       <c r="A18" s="43" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
@@ -3252,7 +3329,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G20" s="17"/>
       <c r="AC20" s="27"/>
@@ -3267,33 +3344,33 @@
     <row r="21" spans="1:36" ht="15" customHeight="1">
       <c r="A21" s="56"/>
       <c r="B21" s="66" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C21" s="67"/>
       <c r="D21" s="68" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E21" s="69"/>
       <c r="F21" s="70"/>
       <c r="G21" s="68" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H21" s="69"/>
       <c r="I21" s="70"/>
       <c r="J21" s="68" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="K21" s="69"/>
       <c r="L21" s="69"/>
       <c r="M21" s="70"/>
       <c r="N21" s="68" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="O21" s="69"/>
       <c r="P21" s="69"/>
       <c r="Q21" s="70"/>
       <c r="R21" s="68" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="S21" s="69"/>
       <c r="T21" s="69"/>
@@ -3314,29 +3391,29 @@
       </c>
       <c r="C22" s="71"/>
       <c r="D22" s="72" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E22" s="71"/>
       <c r="F22" s="59"/>
       <c r="G22" s="72" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H22" s="71"/>
       <c r="I22" s="59"/>
       <c r="J22" s="72" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="K22" s="71"/>
       <c r="L22" s="71"/>
       <c r="M22" s="59"/>
       <c r="N22" s="72" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="O22" s="71"/>
       <c r="P22" s="71"/>
       <c r="Q22" s="59"/>
       <c r="R22" s="72" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="S22" s="71"/>
       <c r="T22" s="71"/>
@@ -3356,23 +3433,23 @@
       </c>
       <c r="C23" s="71"/>
       <c r="D23" s="72" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E23" s="71"/>
       <c r="F23" s="59"/>
       <c r="G23" s="72" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="H23" s="71"/>
       <c r="I23" s="59"/>
       <c r="J23" s="72" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="K23" s="71"/>
       <c r="L23" s="71"/>
       <c r="M23" s="59"/>
       <c r="N23" s="72" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="O23" s="71"/>
       <c r="P23" s="71"/>
@@ -3380,7 +3457,7 @@
       <c r="R23" s="72"/>
       <c r="S23" s="71"/>
       <c r="T23" s="71" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="U23" s="59"/>
       <c r="AC23" s="61"/>
@@ -3398,23 +3475,23 @@
       </c>
       <c r="C24" s="71"/>
       <c r="D24" s="72" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E24" s="71"/>
       <c r="F24" s="59"/>
       <c r="G24" s="72" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H24" s="71"/>
       <c r="I24" s="59"/>
       <c r="J24" s="72" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="K24" s="71"/>
       <c r="L24" s="71"/>
       <c r="M24" s="59"/>
       <c r="N24" s="72" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="O24" s="71"/>
       <c r="P24" s="71"/>
@@ -3422,7 +3499,7 @@
       <c r="R24" s="72"/>
       <c r="S24" s="71"/>
       <c r="T24" s="71" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="U24" s="59"/>
       <c r="AC24" s="61"/>
@@ -3440,29 +3517,29 @@
       </c>
       <c r="C25" s="71"/>
       <c r="D25" s="72" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E25" s="71"/>
       <c r="F25" s="59"/>
       <c r="G25" s="72" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="H25" s="71"/>
       <c r="I25" s="59"/>
       <c r="J25" s="72" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="K25" s="71"/>
       <c r="L25" s="71"/>
       <c r="M25" s="59"/>
       <c r="N25" s="72" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="O25" s="71"/>
       <c r="P25" s="71"/>
       <c r="Q25" s="59"/>
       <c r="R25" s="72" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="S25" s="71"/>
       <c r="T25" s="71"/>
@@ -3483,23 +3560,23 @@
       </c>
       <c r="C26" s="71"/>
       <c r="D26" s="72" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E26" s="71"/>
       <c r="F26" s="59"/>
       <c r="G26" s="72" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H26" s="71"/>
       <c r="I26" s="59"/>
       <c r="J26" s="72" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="K26" s="71"/>
       <c r="L26" s="71"/>
       <c r="M26" s="59"/>
       <c r="N26" s="72" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="O26" s="71"/>
       <c r="P26" s="71"/>
@@ -3507,7 +3584,7 @@
       <c r="R26" s="72"/>
       <c r="S26" s="71"/>
       <c r="T26" s="71" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="U26" s="59"/>
       <c r="AC26" s="61"/>
@@ -3521,6 +3598,28 @@
     </row>
     <row r="27" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="60"/>
+      <c r="B27" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="41"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="110"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="110"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
       <c r="AC27" s="61"/>
       <c r="AD27" s="62"/>
       <c r="AE27" s="63"/>
@@ -3532,6 +3631,9 @@
     </row>
     <row r="28" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="60"/>
+      <c r="B28" s="44" t="s">
+        <v>73</v>
+      </c>
       <c r="AC28" s="61"/>
       <c r="AD28" s="62"/>
       <c r="AE28" s="63"/>
@@ -3543,6 +3645,9 @@
     </row>
     <row r="29" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A29" s="60"/>
+      <c r="B29" s="44" t="s">
+        <v>74</v>
+      </c>
       <c r="AC29" s="61"/>
       <c r="AD29" s="62"/>
       <c r="AE29" s="63"/>
@@ -3575,7 +3680,9 @@
       <c r="AJ31" s="61"/>
     </row>
     <row r="32" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A32" s="60"/>
+      <c r="A32" s="65" t="s">
+        <v>76</v>
+      </c>
       <c r="AC32" s="61"/>
       <c r="AD32" s="62"/>
       <c r="AE32" s="63"/>
@@ -3586,7 +3693,12 @@
       <c r="AJ32" s="61"/>
     </row>
     <row r="33" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="60"/>
+      <c r="A33" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>77</v>
+      </c>
       <c r="AC33" s="61"/>
       <c r="AD33" s="62"/>
       <c r="AE33" s="63"/>
@@ -3598,6 +3710,18 @@
     </row>
     <row r="34" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A34" s="60"/>
+      <c r="B34" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="69"/>
+      <c r="I34" s="70"/>
       <c r="AC34" s="61"/>
       <c r="AD34" s="62"/>
       <c r="AE34" s="63"/>
@@ -3609,6 +3733,18 @@
     </row>
     <row r="35" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A35" s="60"/>
+      <c r="B35" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="H35" s="71"/>
+      <c r="I35" s="59"/>
       <c r="AC35" s="61"/>
       <c r="AD35" s="62"/>
       <c r="AE35" s="63"/>
@@ -3620,6 +3756,18 @@
     </row>
     <row r="36" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A36" s="60"/>
+      <c r="B36" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="H36" s="71"/>
+      <c r="I36" s="59"/>
       <c r="AC36" s="61"/>
       <c r="AD36" s="62"/>
       <c r="AE36" s="63"/>
@@ -3631,6 +3779,18 @@
     </row>
     <row r="37" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A37" s="60"/>
+      <c r="B37" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37" s="71"/>
+      <c r="I37" s="59"/>
       <c r="AC37" s="61"/>
       <c r="AD37" s="62"/>
       <c r="AE37" s="63"/>
@@ -3642,6 +3802,18 @@
     </row>
     <row r="38" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A38" s="60"/>
+      <c r="B38" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38" s="71"/>
+      <c r="I38" s="59"/>
       <c r="AC38" s="61"/>
       <c r="AD38" s="62"/>
       <c r="AE38" s="63"/>
@@ -3674,7 +3846,9 @@
       <c r="AJ40" s="61"/>
     </row>
     <row r="41" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="60"/>
+      <c r="A41" s="65" t="s">
+        <v>87</v>
+      </c>
       <c r="AC41" s="61"/>
       <c r="AD41" s="62"/>
       <c r="AE41" s="63"/>
@@ -3685,7 +3859,12 @@
       <c r="AJ41" s="61"/>
     </row>
     <row r="42" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="60"/>
+      <c r="A42" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="44" t="s">
+        <v>88</v>
+      </c>
       <c r="AC42" s="61"/>
       <c r="AD42" s="62"/>
       <c r="AE42" s="63"/>
@@ -3707,7 +3886,12 @@
       <c r="AJ43" s="61"/>
     </row>
     <row r="44" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A44" s="60"/>
+      <c r="A44" s="111" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>91</v>
+      </c>
       <c r="AC44" s="61"/>
       <c r="AD44" s="62"/>
       <c r="AE44" s="63"/>
@@ -3719,6 +3903,9 @@
     </row>
     <row r="45" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A45" s="60"/>
+      <c r="B45" s="44" t="s">
+        <v>90</v>
+      </c>
       <c r="AC45" s="61"/>
       <c r="AD45" s="62"/>
       <c r="AE45" s="63"/>
@@ -3730,6 +3917,9 @@
     </row>
     <row r="46" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A46" s="60"/>
+      <c r="C46" s="44" t="s">
+        <v>92</v>
+      </c>
       <c r="AC46" s="61"/>
       <c r="AD46" s="62"/>
       <c r="AE46" s="63"/>
@@ -3741,6 +3931,9 @@
     </row>
     <row r="47" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A47" s="60"/>
+      <c r="B47" s="44" t="s">
+        <v>93</v>
+      </c>
       <c r="AC47" s="61"/>
       <c r="AD47" s="62"/>
       <c r="AE47" s="63"/>
@@ -3752,6 +3945,9 @@
     </row>
     <row r="48" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A48" s="60"/>
+      <c r="C48" s="44" t="s">
+        <v>94</v>
+      </c>
       <c r="AC48" s="61"/>
       <c r="AD48" s="62"/>
       <c r="AE48" s="63"/>
@@ -3763,6 +3959,9 @@
     </row>
     <row r="49" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
       <c r="A49" s="60"/>
+      <c r="C49" s="44" t="s">
+        <v>95</v>
+      </c>
       <c r="AC49" s="61"/>
       <c r="AD49" s="62"/>
       <c r="AE49" s="63"/>
@@ -3795,7 +3994,9 @@
       <c r="AJ51" s="61"/>
     </row>
     <row r="52" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A52" s="60"/>
+      <c r="A52" s="65" t="s">
+        <v>96</v>
+      </c>
       <c r="AC52" s="61"/>
       <c r="AD52" s="62"/>
       <c r="AE52" s="63"/>
@@ -3806,7 +4007,12 @@
       <c r="AJ52" s="61"/>
     </row>
     <row r="53" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A53" s="60"/>
+      <c r="A53" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" s="44" t="s">
+        <v>98</v>
+      </c>
       <c r="AC53" s="61"/>
       <c r="AD53" s="62"/>
       <c r="AE53" s="63"/>
@@ -3817,7 +4023,12 @@
       <c r="AJ53" s="61"/>
     </row>
     <row r="54" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A54" s="60"/>
+      <c r="A54" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>99</v>
+      </c>
       <c r="AC54" s="61"/>
       <c r="AD54" s="62"/>
       <c r="AE54" s="63"/>
@@ -3838,245 +4049,43 @@
       <c r="AI55" s="63"/>
       <c r="AJ55" s="61"/>
     </row>
-    <row r="56" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A56" s="60"/>
-      <c r="AC56" s="61"/>
-      <c r="AD56" s="62"/>
-      <c r="AE56" s="63"/>
-      <c r="AF56" s="63"/>
-      <c r="AG56" s="63"/>
-      <c r="AH56" s="63"/>
-      <c r="AI56" s="63"/>
-      <c r="AJ56" s="61"/>
-    </row>
-    <row r="57" spans="1:36" ht="15" customHeight="1">
-      <c r="A57" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G57" s="17"/>
-      <c r="AC57" s="27"/>
-      <c r="AD57" s="26"/>
-      <c r="AE57" s="41"/>
-      <c r="AF57" s="41"/>
-      <c r="AG57" s="41"/>
-      <c r="AH57" s="41"/>
-      <c r="AI57" s="41"/>
-      <c r="AJ57" s="27"/>
-    </row>
-    <row r="58" spans="1:36" ht="15" customHeight="1">
-      <c r="A58" s="56"/>
-      <c r="B58" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G58" s="17"/>
-      <c r="AC58" s="27"/>
-      <c r="AD58" s="26"/>
-      <c r="AE58" s="41"/>
-      <c r="AF58" s="41"/>
-      <c r="AG58" s="41"/>
-      <c r="AH58" s="41"/>
-      <c r="AI58" s="41"/>
-      <c r="AJ58" s="27"/>
-    </row>
-    <row r="59" spans="1:36" ht="15" customHeight="1">
-      <c r="A59" s="56"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G59" s="17"/>
-      <c r="AC59" s="27"/>
-      <c r="AD59" s="26"/>
-      <c r="AE59" s="41"/>
-      <c r="AF59" s="41"/>
-      <c r="AG59" s="41"/>
-      <c r="AH59" s="41"/>
-      <c r="AI59" s="41"/>
-      <c r="AJ59" s="27"/>
-    </row>
-    <row r="60" spans="1:36" ht="15" customHeight="1">
-      <c r="A60" s="56"/>
-      <c r="B60" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G60" s="17"/>
-      <c r="AC60" s="27"/>
-      <c r="AD60" s="26"/>
-      <c r="AE60" s="41"/>
-      <c r="AF60" s="41"/>
-      <c r="AG60" s="41"/>
-      <c r="AH60" s="41"/>
-      <c r="AI60" s="41"/>
-      <c r="AJ60" s="27"/>
-    </row>
-    <row r="61" spans="1:36" ht="15" customHeight="1">
-      <c r="A61" s="56"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G61" s="17"/>
-      <c r="AC61" s="27"/>
-      <c r="AD61" s="26"/>
-      <c r="AE61" s="41"/>
-      <c r="AF61" s="41"/>
-      <c r="AG61" s="41"/>
-      <c r="AH61" s="41"/>
-      <c r="AI61" s="41"/>
-      <c r="AJ61" s="27"/>
-    </row>
-    <row r="62" spans="1:36" ht="15" customHeight="1">
-      <c r="A62" s="56"/>
-      <c r="B62" s="17"/>
-      <c r="D62" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G62" s="17"/>
-      <c r="AC62" s="27"/>
-      <c r="AD62" s="26"/>
-      <c r="AE62" s="41"/>
-      <c r="AF62" s="41"/>
-      <c r="AG62" s="41"/>
-      <c r="AH62" s="41"/>
-      <c r="AI62" s="41"/>
-      <c r="AJ62" s="27"/>
-    </row>
-    <row r="63" spans="1:36" ht="15" customHeight="1">
-      <c r="A63" s="56"/>
-      <c r="B63" s="17"/>
-      <c r="D63" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="G63" s="17"/>
-      <c r="AC63" s="27"/>
-      <c r="AD63" s="26"/>
-      <c r="AE63" s="41"/>
-      <c r="AF63" s="41"/>
-      <c r="AG63" s="41"/>
-      <c r="AH63" s="41"/>
-      <c r="AI63" s="41"/>
-      <c r="AJ63" s="27"/>
-    </row>
-    <row r="64" spans="1:36" ht="15" customHeight="1">
-      <c r="A64" s="56"/>
-      <c r="B64" s="17"/>
-      <c r="D64" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="G64" s="17"/>
-      <c r="AC64" s="27"/>
-      <c r="AD64" s="26"/>
-      <c r="AE64" s="41"/>
-      <c r="AF64" s="41"/>
-      <c r="AG64" s="41"/>
-      <c r="AH64" s="41"/>
-      <c r="AI64" s="41"/>
-      <c r="AJ64" s="27"/>
-    </row>
-    <row r="65" spans="1:36" ht="15" customHeight="1">
-      <c r="A65" s="56"/>
-      <c r="B65" s="17"/>
-      <c r="D65" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="G65" s="17"/>
-      <c r="AC65" s="27"/>
-      <c r="AD65" s="26"/>
-      <c r="AE65" s="41"/>
-      <c r="AF65" s="41"/>
-      <c r="AG65" s="41"/>
-      <c r="AH65" s="41"/>
-      <c r="AI65" s="41"/>
-      <c r="AJ65" s="27"/>
-    </row>
-    <row r="66" spans="1:36" ht="15" customHeight="1">
-      <c r="A66" s="56"/>
-      <c r="B66" s="17"/>
-      <c r="D66" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="G66" s="17"/>
-      <c r="AC66" s="27"/>
-      <c r="AD66" s="26"/>
-      <c r="AE66" s="41"/>
-      <c r="AF66" s="41"/>
-      <c r="AG66" s="41"/>
-      <c r="AH66" s="41"/>
-      <c r="AI66" s="41"/>
-      <c r="AJ66" s="27"/>
-    </row>
-    <row r="67" spans="1:36" ht="15" customHeight="1">
-      <c r="A67" s="56"/>
-      <c r="B67" s="17"/>
-      <c r="D67" s="44"/>
-      <c r="E67" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="F67" s="65"/>
-      <c r="G67" s="65"/>
-      <c r="H67" s="65"/>
-      <c r="I67" s="65"/>
-      <c r="J67" s="65"/>
-      <c r="AC67" s="27"/>
-      <c r="AD67" s="26"/>
-      <c r="AE67" s="41"/>
-      <c r="AF67" s="41"/>
-      <c r="AG67" s="41"/>
-      <c r="AH67" s="41"/>
-      <c r="AI67" s="41"/>
-      <c r="AJ67" s="27"/>
-    </row>
-    <row r="68" spans="1:36" s="44" customFormat="1" ht="15" customHeight="1">
-      <c r="A68" s="60"/>
-      <c r="AC68" s="61"/>
-      <c r="AD68" s="62"/>
-      <c r="AE68" s="63"/>
-      <c r="AF68" s="63"/>
-      <c r="AG68" s="63"/>
-      <c r="AH68" s="63"/>
-      <c r="AI68" s="63"/>
-      <c r="AJ68" s="61"/>
-    </row>
-    <row r="69" spans="1:36" ht="15" customHeight="1">
-      <c r="A69" s="57"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="30"/>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30"/>
-      <c r="K69" s="30"/>
-      <c r="L69" s="30"/>
-      <c r="M69" s="30"/>
-      <c r="N69" s="30"/>
-      <c r="O69" s="30"/>
-      <c r="P69" s="30"/>
-      <c r="Q69" s="30"/>
-      <c r="R69" s="30"/>
-      <c r="S69" s="30"/>
-      <c r="T69" s="30"/>
-      <c r="U69" s="30"/>
-      <c r="V69" s="30"/>
-      <c r="W69" s="30"/>
-      <c r="X69" s="30"/>
-      <c r="Y69" s="30"/>
-      <c r="Z69" s="30"/>
-      <c r="AA69" s="30"/>
-      <c r="AB69" s="30"/>
-      <c r="AC69" s="31"/>
-      <c r="AD69" s="28"/>
-      <c r="AE69" s="30"/>
-      <c r="AF69" s="30"/>
-      <c r="AG69" s="30"/>
-      <c r="AH69" s="30"/>
-      <c r="AI69" s="30"/>
-      <c r="AJ69" s="31"/>
+    <row r="56" spans="1:36" ht="15" customHeight="1">
+      <c r="A56" s="57"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="30"/>
+      <c r="K56" s="30"/>
+      <c r="L56" s="30"/>
+      <c r="M56" s="30"/>
+      <c r="N56" s="30"/>
+      <c r="O56" s="30"/>
+      <c r="P56" s="30"/>
+      <c r="Q56" s="30"/>
+      <c r="R56" s="30"/>
+      <c r="S56" s="30"/>
+      <c r="T56" s="30"/>
+      <c r="U56" s="30"/>
+      <c r="V56" s="30"/>
+      <c r="W56" s="30"/>
+      <c r="X56" s="30"/>
+      <c r="Y56" s="30"/>
+      <c r="Z56" s="30"/>
+      <c r="AA56" s="30"/>
+      <c r="AB56" s="30"/>
+      <c r="AC56" s="31"/>
+      <c r="AD56" s="28"/>
+      <c r="AE56" s="30"/>
+      <c r="AF56" s="30"/>
+      <c r="AG56" s="30"/>
+      <c r="AH56" s="30"/>
+      <c r="AI56" s="30"/>
+      <c r="AJ56" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>